<commit_message>
Updated README.ja and added examples
</commit_message>
<xml_diff>
--- a/testfiles/newPresidents.xlsx
+++ b/testfiles/newPresidents.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\workspace\exceltable\xlbean\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="8230" windowWidth="19200" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="presidents" r:id="rId1" sheetId="7"/>
+    <sheet name="presidents" sheetId="7" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>####</t>
     <phoneticPr fontId="1"/>
@@ -177,11 +177,15 @@
   <si>
     <t>New York</t>
   </si>
+  <si>
+    <t>United States of America</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="177" formatCode="_-\$* #,##0.00_ ;_-\$* \-#,##0.00\ ;_-\$* &quot;-&quot;??_ ;_-@_ "/>
@@ -382,65 +386,65 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="14" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="176" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="4" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="5" fillId="0" fontId="3" numFmtId="177" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="6" fillId="0" fontId="3" numFmtId="177" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="1" applyFont="1" borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="1" applyFont="1" borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="標準" xfId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -457,9 +461,10 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Helvetica"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt formatCode="@" numFmtId="30"/>
+      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
     </dxf>
     <dxf>
       <font>
@@ -478,7 +483,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt formatCode="0_);[Red]\(0\)" numFmtId="176"/>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
     </dxf>
     <dxf>
       <font>
@@ -497,7 +502,25 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt formatCode="yyyy/m/d" numFmtId="19"/>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -516,7 +539,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt formatCode="yyyy/m/d" numFmtId="19"/>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
     </dxf>
     <dxf>
       <font>
@@ -535,26 +558,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt formatCode="yyyy/m/d" numFmtId="19"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt formatCode="@" numFmtId="30"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -593,7 +597,7 @@
       </font>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -606,17 +610,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="6" displayName="テーブル4" headerRowDxfId="7" id="4" name="テーブル4" ref="C7:H18" totalsRowShown="0">
-  <autoFilter ref="C7:H18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="テーブル4" displayName="テーブル4" ref="C7:H18" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="C7:H18" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="6">
-    <tableColumn dataDxfId="5" id="1" name="Name"/>
-    <tableColumn dataDxfId="4" id="2" name="Date of birth"/>
-    <tableColumn dataDxfId="0" id="3" name="State of birth"/>
-    <tableColumn dataDxfId="3" id="4" name="In office from"/>
-    <tableColumn dataDxfId="2" id="5" name="In office to"/>
-    <tableColumn dataDxfId="1" id="6" name="# of days _x000a_in office"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Date of birth" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="State of birth" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="In office from" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="In office to" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="# of days _x000a_in office" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -625,10 +629,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -663,7 +667,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -715,7 +719,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -826,21 +830,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -857,7 +861,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -909,30 +913,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:E18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="13.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="1" width="2.33203125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="17.58203125" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="48.58203125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="1" width="15.33203125" collapsed="false"/>
-    <col min="6" max="7" customWidth="true" style="1" width="12.75" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" style="1" width="12.1640625" collapsed="false"/>
-    <col min="9" max="16384" style="1" width="8.6640625" collapsed="false"/>
+    <col min="1" max="1" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="12.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -958,7 +960,7 @@
         <v>12</v>
       </c>
     </row>
-    <row ht="14.5" r="2" spans="1:8" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8" t="s">
         <v>17</v>
@@ -966,7 +968,9 @@
       <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -976,20 +980,24 @@
       <c r="C4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-    </row>
-    <row ht="14.5" r="5" spans="1:8" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="D4" s="16">
+        <v>9628000</v>
+      </c>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="13">
+        <v>15653300000000</v>
+      </c>
       <c r="E5" s="14"/>
     </row>
-    <row ht="28" r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" ht="28" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1016,218 +1024,218 @@
       <c r="C8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="2" t="n">
-        <v>6359.0</v>
+      <c r="D8" s="2">
+        <v>6359</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="2" t="n">
-        <v>22301.0</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>23337.0</v>
-      </c>
-      <c r="H8" s="4" t="n">
-        <v>1036.0</v>
+      <c r="F8" s="2">
+        <v>22301</v>
+      </c>
+      <c r="G8" s="2">
+        <v>23337</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1036</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="2" t="n">
-        <v>3162.0</v>
+      <c r="D9" s="2">
+        <v>3162</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="2" t="n">
-        <v>23337.0</v>
-      </c>
-      <c r="G9" s="2" t="n">
-        <v>25223.0</v>
-      </c>
-      <c r="H9" s="4" t="n">
-        <v>1886.0</v>
+      <c r="F9" s="2">
+        <v>23337</v>
+      </c>
+      <c r="G9" s="2">
+        <v>25223</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1886</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="2" t="n">
-        <v>4758.0</v>
+      <c r="D10" s="2">
+        <v>4758</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="2" t="n">
-        <v>25223.0</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>27250.0</v>
-      </c>
-      <c r="H10" s="4" t="n">
-        <v>2027.0</v>
+      <c r="F10" s="2">
+        <v>25223</v>
+      </c>
+      <c r="G10" s="2">
+        <v>27250</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2027</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="2" t="n">
-        <v>4944.0</v>
+      <c r="D11" s="2">
+        <v>4944</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="2" t="n">
-        <v>27250.0</v>
-      </c>
-      <c r="G11" s="2" t="n">
-        <v>28145.0</v>
-      </c>
-      <c r="H11" s="4" t="n">
-        <v>895.0</v>
+      <c r="F11" s="2">
+        <v>27250</v>
+      </c>
+      <c r="G11" s="2">
+        <v>28145</v>
+      </c>
+      <c r="H11" s="4">
+        <v>895</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="2" t="n">
-        <v>9041.0</v>
+      <c r="D12" s="2">
+        <v>9041</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="2" t="n">
-        <v>28145.0</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>29606.0</v>
-      </c>
-      <c r="H12" s="4" t="n">
-        <v>1461.0</v>
+      <c r="F12" s="2">
+        <v>28145</v>
+      </c>
+      <c r="G12" s="2">
+        <v>29606</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1461</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="2" t="n">
-        <v>4055.0</v>
+      <c r="D13" s="2">
+        <v>4055</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="2" t="n">
-        <v>29606.0</v>
-      </c>
-      <c r="G13" s="2" t="n">
-        <v>32528.0</v>
-      </c>
-      <c r="H13" s="4" t="n">
-        <v>2922.0</v>
+      <c r="F13" s="2">
+        <v>29606</v>
+      </c>
+      <c r="G13" s="2">
+        <v>32528</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2922</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="2" t="n">
-        <v>8930.0</v>
+      <c r="D14" s="2">
+        <v>8930</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="2" t="n">
-        <v>32528.0</v>
-      </c>
-      <c r="G14" s="2" t="n">
-        <v>33989.0</v>
-      </c>
-      <c r="H14" s="4" t="n">
-        <v>1461.0</v>
+      <c r="F14" s="2">
+        <v>32528</v>
+      </c>
+      <c r="G14" s="2">
+        <v>33989</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1461</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="2" t="n">
-        <v>17033.0</v>
+      <c r="D15" s="2">
+        <v>17033</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="2" t="n">
-        <v>33989.0</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>36911.0</v>
-      </c>
-      <c r="H15" s="4" t="n">
-        <v>2922.0</v>
+      <c r="F15" s="2">
+        <v>33989</v>
+      </c>
+      <c r="G15" s="2">
+        <v>36911</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2922</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="2" t="n">
-        <v>16989.0</v>
+      <c r="D16" s="2">
+        <v>16989</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="2" t="n">
-        <v>36911.0</v>
-      </c>
-      <c r="G16" s="2" t="n">
-        <v>39833.0</v>
-      </c>
-      <c r="H16" s="4" t="n">
-        <v>2922.0</v>
+      <c r="F16" s="2">
+        <v>36911</v>
+      </c>
+      <c r="G16" s="2">
+        <v>39833</v>
+      </c>
+      <c r="H16" s="4">
+        <v>2922</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="2" t="n">
-        <v>22497.0</v>
+      <c r="D17" s="2">
+        <v>22497</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="2" t="n">
-        <v>39833.0</v>
-      </c>
-      <c r="G17" s="2" t="n">
-        <v>42755.0</v>
-      </c>
-      <c r="H17" s="4" t="n">
-        <v>2922.0</v>
+      <c r="F17" s="2">
+        <v>39833</v>
+      </c>
+      <c r="G17" s="2">
+        <v>42755</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2922</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="2" t="n">
-        <v>16967.0</v>
+      <c r="D18" s="2">
+        <v>16967</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="2" t="n">
-        <v>42755.0</v>
+      <c r="F18" s="2">
+        <v>42755</v>
       </c>
       <c r="G18" s="2"/>
-      <c r="H18" s="4" t="n">
-        <v>0.0</v>
+      <c r="H18" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1237,8 +1245,8 @@
     <mergeCell ref="D4:E4"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>